<commit_message>
prob 1 mostly working
</commit_message>
<xml_diff>
--- a/hw2/doubleor.xlsx
+++ b/hw2/doubleor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liam_adams/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liam_adams/my_repos/csc_qc/hw2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5F2097-CFA5-A649-857A-961A78DC6BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69149BA-85CE-1A4D-B4E2-89C9FDBDA7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="640" windowWidth="20100" windowHeight="17240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14560" yWindow="460" windowWidth="20100" windowHeight="17240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5qubit" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <r>
       <t>a</t>
@@ -494,6 +494,9 @@
       </rPr>
       <t>6</t>
     </r>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1162,7 +1165,7 @@
         <v>-1</v>
       </c>
       <c r="C2" s="5">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="D2" s="5">
         <v>-1</v>
@@ -1375,9 +1378,11 @@
       </c>
       <c r="H9" s="12">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="I9" s="9"/>
+        <v>-2</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="8"/>
@@ -1403,7 +1408,7 @@
       </c>
       <c r="H10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -1431,9 +1436,11 @@
       </c>
       <c r="H11" s="12">
         <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="I11" s="9"/>
+        <v>-2</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="8"/>
@@ -1459,7 +1466,7 @@
       </c>
       <c r="H12" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1517,7 +1524,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="8"/>
@@ -1545,7 +1554,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="8"/>
@@ -1599,7 +1610,7 @@
       </c>
       <c r="H17" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -1627,7 +1638,7 @@
       </c>
       <c r="H18" s="12">
         <f>A$2*C18+B$2*D18+C$2*E18+D$2*F18+E$2*G18+F$2*C18*D18+G$2*C18*E18+H$2*C18*F18+I$2*C18*G18+J$2*D18*E18+K$2*D18*F18+L$2*D18*G18+M$2*E18*F18+N$2*E18*G18+O$2*F18*G18</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -1655,7 +1666,7 @@
       </c>
       <c r="H19" s="12">
         <f>A$2*C19+B$2*D19+C$2*E19+D$2*F19+E$2*G19+F$2*C19*D19+G$2*C19*E19+H$2*C19*F19+I$2*C19*G19+J$2*D19*E19+K$2*D19*F19+L$2*D19*G19+M$2*E19*F19+N$2*E19*G19+O$2*F19*G19</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -1683,7 +1694,7 @@
       </c>
       <c r="H20" s="12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -1741,7 +1752,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -1769,7 +1782,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J23" s="9"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
@@ -1823,7 +1838,7 @@
       </c>
       <c r="H25" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -1851,7 +1866,7 @@
       </c>
       <c r="H26" s="12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -1879,7 +1894,7 @@
       </c>
       <c r="H27" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -1907,7 +1922,7 @@
       </c>
       <c r="H28" s="12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -1965,7 +1980,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J30" s="9"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
@@ -1993,7 +2010,9 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="J31" s="9"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
@@ -2047,7 +2066,7 @@
       </c>
       <c r="H33" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -2075,7 +2094,7 @@
       </c>
       <c r="H34" s="12">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="9"/>
       <c r="J34" s="9"/>
@@ -2103,7 +2122,7 @@
       </c>
       <c r="H35" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
@@ -2131,7 +2150,7 @@
       </c>
       <c r="H36" s="12">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
@@ -2152,10 +2171,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1740" topLeftCell="A31" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1740" activePane="bottomLeft"/>
       <selection activeCell="U2" sqref="U2"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2227,28 +2246,28 @@
     </row>
     <row r="2" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B2" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="E2" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2" s="5">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="5">
         <v>0</v>
@@ -2263,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="M2" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N2" s="5">
         <v>0</v>
@@ -2272,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Q2" s="7">
         <v>0</v>
@@ -2281,13 +2300,13 @@
         <v>0</v>
       </c>
       <c r="S2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T2" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U2" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -2386,7 +2405,7 @@
       </c>
       <c r="H6" s="12">
         <f t="shared" ref="H6:H36" si="0">A$2*B6+B$2*C6+C$2*D6+D$2*E6+E$2*F6+F$2*G6+G$2*B6*C6+H$2*B6*D6+I$2*B6*E6+J$2*B6*F6+K$2*B6*G6+L$2*C6*D6+M$2*C6*E6+N$2*C6*F6+O$2*C6*G6+P$2*D6*E6+Q$2*D6*F6+R$2*D6*G6+S$2*E6*F6+T$2*E6*G6+U$2*F6*G6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -2416,7 +2435,7 @@
       </c>
       <c r="H7" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -2476,7 +2495,7 @@
       </c>
       <c r="H9" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -2506,7 +2525,7 @@
       </c>
       <c r="H10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -2536,7 +2555,7 @@
       </c>
       <c r="H11" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -2566,7 +2585,7 @@
       </c>
       <c r="H12" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -2596,7 +2615,7 @@
       </c>
       <c r="H13" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -2626,7 +2645,7 @@
       </c>
       <c r="H14" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -2656,7 +2675,7 @@
       </c>
       <c r="H15" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -2686,7 +2705,7 @@
       </c>
       <c r="H16" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -2716,7 +2735,7 @@
       </c>
       <c r="H17" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
@@ -2746,7 +2765,7 @@
       </c>
       <c r="H18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -2776,7 +2795,7 @@
       </c>
       <c r="H19" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -2806,7 +2825,7 @@
       </c>
       <c r="H20" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -2836,7 +2855,7 @@
       </c>
       <c r="H21" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -2866,7 +2885,7 @@
       </c>
       <c r="H22" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -2896,7 +2915,7 @@
       </c>
       <c r="H23" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -2926,7 +2945,7 @@
       </c>
       <c r="H24" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -2956,7 +2975,7 @@
       </c>
       <c r="H25" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -2986,7 +3005,7 @@
       </c>
       <c r="H26" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -3016,7 +3035,7 @@
       </c>
       <c r="H27" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -3046,7 +3065,7 @@
       </c>
       <c r="H28" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
@@ -3076,7 +3095,7 @@
       </c>
       <c r="H29" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
@@ -3106,7 +3125,7 @@
       </c>
       <c r="H30" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
@@ -3136,7 +3155,7 @@
       </c>
       <c r="H31" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
@@ -3166,7 +3185,7 @@
       </c>
       <c r="H32" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
@@ -3196,7 +3215,7 @@
       </c>
       <c r="H33" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -3256,7 +3275,7 @@
       </c>
       <c r="H35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
@@ -3286,7 +3305,7 @@
       </c>
       <c r="H36" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36" s="9"/>
       <c r="J36" s="9"/>
@@ -3316,7 +3335,7 @@
       </c>
       <c r="H37" s="12">
         <f>A$2*B37+B$2*C37+C$2*D37+D$2*E37+E$2*F37+F$2*G37+G$2*B37*C37+H$2*B37*D37+I$2*B37*E37+J$2*B37*F37+K$2*B37*G37+L$2*C37*D37+M$2*C37*E37+N$2*C37*F37+O$2*C37*G37+P$2*D37*E37+Q$2*D37*F37+R$2*D37*G37+S$2*E37*F37+T$2*E37*G37+U$2*F37*G37</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9"/>
@@ -3346,7 +3365,7 @@
       </c>
       <c r="H38" s="12">
         <f t="shared" ref="H38:H68" si="1">A$2*B38+B$2*C38+C$2*D38+D$2*E38+E$2*F38+F$2*G38+G$2*B38*C38+H$2*B38*D38+I$2*B38*E38+J$2*B38*F38+K$2*B38*G38+L$2*C38*D38+M$2*C38*E38+N$2*C38*F38+O$2*C38*G38+P$2*D38*E38+Q$2*D38*F38+R$2*D38*G38+S$2*E38*F38+T$2*E38*G38+U$2*F38*G38</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
@@ -3376,7 +3395,7 @@
       </c>
       <c r="H39" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
@@ -3406,7 +3425,7 @@
       </c>
       <c r="H40" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I40" s="9"/>
       <c r="J40" s="9"/>
@@ -3436,7 +3455,7 @@
       </c>
       <c r="H41" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
@@ -3466,7 +3485,7 @@
       </c>
       <c r="H42" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
@@ -3496,7 +3515,7 @@
       </c>
       <c r="H43" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
@@ -3526,7 +3545,7 @@
       </c>
       <c r="H44" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
@@ -3556,7 +3575,7 @@
       </c>
       <c r="H45" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
@@ -3586,7 +3605,7 @@
       </c>
       <c r="H46" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
@@ -3616,7 +3635,7 @@
       </c>
       <c r="H47" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
@@ -3646,7 +3665,7 @@
       </c>
       <c r="H48" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
@@ -3676,7 +3695,7 @@
       </c>
       <c r="H49" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
@@ -3736,7 +3755,7 @@
       </c>
       <c r="H51" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
@@ -3766,7 +3785,7 @@
       </c>
       <c r="H52" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
@@ -3796,7 +3815,7 @@
       </c>
       <c r="H53" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
@@ -3826,7 +3845,7 @@
       </c>
       <c r="H54" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
@@ -3856,7 +3875,7 @@
       </c>
       <c r="H55" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
@@ -3886,7 +3905,7 @@
       </c>
       <c r="H56" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
@@ -3916,7 +3935,7 @@
       </c>
       <c r="H57" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
@@ -3946,7 +3965,7 @@
       </c>
       <c r="H58" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
@@ -3976,7 +3995,7 @@
       </c>
       <c r="H59" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
@@ -4006,7 +4025,7 @@
       </c>
       <c r="H60" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
@@ -4036,7 +4055,7 @@
       </c>
       <c r="H61" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
@@ -4066,7 +4085,7 @@
       </c>
       <c r="H62" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
@@ -4096,7 +4115,7 @@
       </c>
       <c r="H63" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
@@ -4126,7 +4145,7 @@
       </c>
       <c r="H64" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
@@ -4156,7 +4175,7 @@
       </c>
       <c r="H65" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
@@ -4186,7 +4205,7 @@
       </c>
       <c r="H66" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
@@ -4216,7 +4235,7 @@
       </c>
       <c r="H67" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
@@ -4246,7 +4265,7 @@
       </c>
       <c r="H68" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>

</xml_diff>